<commit_message>
Retirei o acento da palavra Cenário
</commit_message>
<xml_diff>
--- a/Ferramenta - Sabrina.xlsx
+++ b/Ferramenta - Sabrina.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\i437543\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabri\Documents\GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{114E3BE7-BEED-4C1A-AB2E-74CEDFEB6E67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8843B11F-9C98-463F-98A6-A60544DED2BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{8DBCBC0D-027F-446D-8F3E-AE09F72996C6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8DBCBC0D-027F-446D-8F3E-AE09F72996C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -37,17 +37,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -82,9 +71,6 @@
     <t>PREMISSAS</t>
   </si>
   <si>
-    <t>Cenários</t>
-  </si>
-  <si>
     <t>Valor Acumulado</t>
   </si>
   <si>
@@ -164,6 +150,9 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Cenarios</t>
   </si>
 </sst>
 </file>
@@ -175,7 +164,7 @@
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -748,6 +737,39 @@
     <xf numFmtId="164" fontId="6" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -779,39 +801,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -2225,129 +2214,129 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E569B1E-A78A-4C3A-AEC4-FF3D47092945}">
   <dimension ref="A8:F39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScale="81" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="81" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7265625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.69921875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.69921875" style="1" customWidth="1"/>
     <col min="6" max="6" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.7265625" style="1" hidden="1"/>
+    <col min="7" max="16384" width="8.69921875" style="1" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="1:4" ht="14.5" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:4" ht="21.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="50" t="s">
+    <row r="8" spans="1:4" ht="14.4" thickBot="1"/>
+    <row r="9" spans="1:4" ht="22.2" thickTop="1" thickBot="1">
+      <c r="B9" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="51"/>
-      <c r="D9" s="52"/>
-    </row>
-    <row r="10" spans="1:4" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="39" t="s">
+      <c r="C9" s="40"/>
+      <c r="D9" s="41"/>
+    </row>
+    <row r="10" spans="1:4" ht="14.4" thickTop="1">
+      <c r="B10" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="45"/>
+      <c r="C10" s="56"/>
       <c r="D10" s="4">
         <v>3400</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B11" s="46" t="s">
+    <row r="11" spans="1:4">
+      <c r="B11" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="47"/>
+      <c r="C11" s="58"/>
       <c r="D11" s="5">
         <v>0.01</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="48" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="49"/>
+    <row r="12" spans="1:4" ht="14.4" thickBot="1">
+      <c r="B12" s="59" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="60"/>
       <c r="D12" s="26">
         <f>Salario*30%</f>
         <v>1020</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:4" ht="35.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="15" thickTop="1" thickBot="1"/>
+    <row r="14" spans="1:4" ht="35.549999999999997" customHeight="1" thickTop="1" thickBot="1">
       <c r="A14" s="6"/>
-      <c r="B14" s="50" t="s">
+      <c r="B14" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="51"/>
-      <c r="D14" s="52"/>
-    </row>
-    <row r="15" spans="1:4" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="57" t="s">
+      <c r="C14" s="40"/>
+      <c r="D14" s="41"/>
+    </row>
+    <row r="15" spans="1:4" ht="14.4" thickTop="1">
+      <c r="B15" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="58"/>
+      <c r="C15" s="47"/>
       <c r="D15" s="7">
         <f>Sugest_Invest</f>
         <v>1020</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B16" s="55" t="s">
+    <row r="16" spans="1:4">
+      <c r="B16" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="56"/>
+      <c r="C16" s="45"/>
       <c r="D16" s="8">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B17" s="55" t="s">
+    <row r="17" spans="2:4">
+      <c r="B17" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="56"/>
+      <c r="C17" s="45"/>
       <c r="D17" s="9">
         <v>0.01</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B18" s="59" t="s">
+    <row r="18" spans="2:4">
+      <c r="B18" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="60"/>
+      <c r="C18" s="49"/>
       <c r="D18" s="10">
         <f>FV(Tx_Rend_Mes,(Por_Qnt_Anos*12),Qtnd_Invest_Mes*-1)</f>
         <v>277333.77331636363</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="43" t="s">
+    <row r="19" spans="2:4" ht="14.4" thickBot="1">
+      <c r="B19" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="44"/>
+      <c r="C19" s="55"/>
       <c r="D19" s="11">
         <f>Patri_Acum*Tx_Rend_Mes</f>
         <v>2773.3377331636361</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="28" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="21" spans="2:4" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:4" ht="28.05" customHeight="1" thickTop="1" thickBot="1"/>
+    <row r="21" spans="2:4" ht="15" thickTop="1" thickBot="1">
       <c r="B21" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="24" t="s">
+      <c r="D21" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="25" t="s">
+    </row>
+    <row r="22" spans="2:4" ht="14.4" thickTop="1">
+      <c r="B22" s="12" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="12" t="s">
-        <v>12</v>
       </c>
       <c r="C22" s="13">
         <f>FV(Rend_Cart,(2*12),Qtnd_Invest_Mes*-1)</f>
@@ -2358,9 +2347,9 @@
         <v>275.1293415025533</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:4">
       <c r="B23" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C23" s="16">
         <f>FV(Rend_Cart,(5*12),Qtnd_Invest_Mes*-1)</f>
@@ -2371,9 +2360,9 @@
         <v>833.03063253537312</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:4">
       <c r="B24" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C24" s="16">
         <f>FV(Rend_Cart,(10*12),Qtnd_Invest_Mes*-1)</f>
@@ -2384,9 +2373,9 @@
         <v>2346.3946324651433</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:4">
       <c r="B25" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C25" s="16">
         <f>FV(Rend_Cart,(20*12),Qtnd_Invest_Mes*-1)</f>
@@ -2397,9 +2386,9 @@
         <v>10090.404726951103</v>
       </c>
     </row>
-    <row r="26" spans="2:4" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:4" ht="14.4" thickBot="1">
       <c r="B26" s="20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C26" s="21">
         <f>FV(Rend_Cart,(30*12),Qtnd_Invest_Mes*-1)</f>
@@ -2410,41 +2399,41 @@
         <v>35648.634154238767</v>
       </c>
     </row>
-    <row r="27" spans="2:4" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="28" spans="2:4" ht="15.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="53" t="s">
+    <row r="27" spans="2:4" ht="15" thickTop="1" thickBot="1"/>
+    <row r="28" spans="2:4" ht="15.45" customHeight="1" thickTop="1" thickBot="1">
+      <c r="B28" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="43"/>
+      <c r="D28" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="54"/>
-      <c r="D28" s="23" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="39" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29" s="40"/>
+    </row>
+    <row r="29" spans="2:4" ht="15" customHeight="1" thickTop="1">
+      <c r="B29" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" s="51"/>
       <c r="D29" s="38">
         <f>Qtnd_Invest_Mes</f>
         <v>1020</v>
       </c>
     </row>
-    <row r="30" spans="2:4" ht="14.5" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="31" spans="2:4" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:4" ht="14.4" thickBot="1"/>
+    <row r="31" spans="2:4" ht="15" thickTop="1" thickBot="1">
       <c r="B31" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" s="25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" ht="14.4" thickTop="1">
+      <c r="B32" s="28" t="s">
         <v>25</v>
-      </c>
-      <c r="C31" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="D31" s="25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="28" t="s">
-        <v>26</v>
       </c>
       <c r="C32" s="31">
         <f>VLOOKUP($D$28&amp;"-"&amp;B32,Planilha2!B4:D21,3,0)</f>
@@ -2455,9 +2444,9 @@
         <v>459</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4">
       <c r="B33" s="29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C33" s="33">
         <f>VLOOKUP($D$28&amp;"-"&amp;B33,Planilha2!B5:D22,3,0)</f>
@@ -2468,9 +2457,9 @@
         <v>357</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:4">
       <c r="B34" s="29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C34" s="33">
         <f>VLOOKUP($D$28&amp;"-"&amp;B34,Planilha2!B6:D23,3,0)</f>
@@ -2481,9 +2470,9 @@
         <v>153</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:4">
       <c r="B35" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C35" s="33">
         <f>VLOOKUP($D$28&amp;"-"&amp;B35,Planilha2!B7:D24,3,0)</f>
@@ -2494,9 +2483,9 @@
         <v>51</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:4">
       <c r="B36" s="29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C36" s="33">
         <f>VLOOKUP($D$28&amp;"-"&amp;B36,Planilha2!B8:D25,3,0)</f>
@@ -2507,9 +2496,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:4" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:4" ht="14.4" thickBot="1">
       <c r="B37" s="30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C37" s="35">
         <f>VLOOKUP($D$28&amp;"-"&amp;B37,Planilha2!B9:D26,3,0)</f>
@@ -2520,19 +2509,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:4" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="C38" s="42"/>
+    <row r="38" spans="2:4" ht="15" thickTop="1" thickBot="1">
+      <c r="B38" s="52" t="s">
+        <v>35</v>
+      </c>
+      <c r="C38" s="53"/>
       <c r="D38" s="37">
         <f>SUM(D32:D37)</f>
         <v>1020</v>
       </c>
     </row>
-    <row r="39" spans="2:4" ht="14.5" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="2:4" ht="14.4" thickTop="1"/>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="B16:C16"/>
@@ -2540,12 +2535,6 @@
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D28" xr:uid="{ED310BF1-F447-49EA-8B06-25318B67234A}">
@@ -2565,238 +2554,238 @@
       <selection activeCell="D16" sqref="D16:D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="2" max="2" width="28.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" style="27"/>
+    <col min="2" max="2" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.09765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.69921875" style="27"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:5">
       <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
         <v>32</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="E3" t="s">
         <v>34</v>
       </c>
-      <c r="E3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="2:5">
       <c r="B4" t="str">
         <f>C4&amp;"-"&amp;Planilha1!B32</f>
         <v>Conservador-PAPEL</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" s="27">
         <v>0.45</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:5">
       <c r="B5" t="str">
         <f>C5&amp;"-"&amp;Planilha1!B33</f>
         <v>Conservador-TIJOLO</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" s="27">
         <v>0.35</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:5">
       <c r="B6" t="str">
         <f>C6&amp;"-"&amp;Planilha1!B34</f>
         <v>Conservador-HIBRIDO</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="27">
         <v>0.15</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:5">
       <c r="B7" t="str">
         <f>C7&amp;"-"&amp;Planilha1!B35</f>
         <v>Conservador-FOFs</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="27">
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:5">
       <c r="B8" t="str">
         <f>C8&amp;"-"&amp;Planilha1!B36</f>
         <v>Conservador-DESENVOLVIMENTO</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" s="27">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:5">
       <c r="B9" t="str">
         <f>C9&amp;"-"&amp;Planilha1!B37</f>
         <v>Conservador-HOTELARIAS</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" s="27">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:5">
       <c r="B10" t="str">
         <f>C10&amp;"-"&amp;Planilha1!B32</f>
         <v>Moderado-PAPEL</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" s="27">
         <v>0.32</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:5">
       <c r="B11" t="str">
         <f>C11&amp;"-"&amp;Planilha1!B33</f>
         <v>Moderado-TIJOLO</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11" s="27">
         <v>0.38</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:5">
       <c r="B12" t="str">
         <f>C12&amp;"-"&amp;Planilha1!B34</f>
         <v>Moderado-HIBRIDO</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D12" s="27">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:5">
       <c r="B13" t="str">
         <f>C13&amp;"-"&amp;Planilha1!B35</f>
         <v>Moderado-FOFs</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D13" s="27">
         <v>0.1</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:5">
       <c r="B14" t="str">
         <f>C14&amp;"-"&amp;Planilha1!B36</f>
         <v>Moderado-DESENVOLVIMENTO</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D14" s="27">
         <v>0.1</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:5">
       <c r="B15" t="str">
         <f>C15&amp;"-"&amp;Planilha1!B37</f>
         <v>Moderado-HOTELARIAS</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D15" s="27">
         <v>0.03</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:5">
       <c r="B16" t="str">
         <f>C16&amp;"-"&amp;Planilha1!B32</f>
         <v>Agressivo-PAPEL</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D16" s="27">
         <v>0.1</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:4">
       <c r="B17" t="str">
         <f>C17&amp;"-"&amp;Planilha1!B33</f>
         <v>Agressivo-TIJOLO</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D17" s="27">
         <v>0.15</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:4">
       <c r="B18" t="str">
         <f>C18&amp;"-"&amp;Planilha1!B34</f>
         <v>Agressivo-HIBRIDO</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D18" s="27">
         <v>0.05</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:4">
       <c r="B19" t="str">
         <f>C19&amp;"-"&amp;Planilha1!B35</f>
         <v>Agressivo-FOFs</v>
       </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D19" s="27">
         <v>0.4</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:4">
       <c r="B20" t="str">
         <f>C20&amp;"-"&amp;Planilha1!B36</f>
         <v>Agressivo-DESENVOLVIMENTO</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D20" s="27">
         <v>0.2</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:4">
       <c r="B21" t="str">
         <f>C21&amp;"-"&amp;Planilha1!B37</f>
         <v>Agressivo-HOTELARIAS</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D21" s="27">
         <v>0.1</v>

</xml_diff>